<commit_message>
Add data Validation to work time
</commit_message>
<xml_diff>
--- a/202302 Табель ОГМ ПК 250.xlsx
+++ b/202302 Табель ОГМ ПК 250.xlsx
@@ -634,16 +634,17 @@
 <file path=xl/comments/comment1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>tc={00970058-00F8-4D6C-BEC0-0051006F00FE}</author>
-    <author>tc={007C0042-00B3-437D-81D2-006800B200FE}</author>
-    <author>tc={00080025-00F5-428C-82C4-009D00930022}</author>
-    <author>tc={00840036-00AD-4C98-A488-003100F9007C}</author>
-    <author>tc={00FD0099-0057-486C-8F18-00F400D000FC}</author>
+    <author>tc={00AB0039-00AB-4733-9704-008800B800EE}</author>
+    <author>tc={00CF0037-00C3-48E1-8630-002A00A200D4}</author>
+    <author>tc={0051005A-00AE-426B-B3E3-007500BF007C}</author>
+    <author>tc={000300BC-0090-4A44-8C2F-00B700C100E6}</author>
+    <author>tc={004200FE-002E-45FF-B273-003E00AE00E9}</author>
   </authors>
   <commentList>
     <comment ref="R16" authorId="0" shapeId="0">
       <text>
-        <t xml:space="preserve">tc={00DE00AF-0057-4E3F-82D1-00B600B700D7}:
+        <t xml:space="preserve">tc={00970058-00F8-4D6C-BEC0-0051006F00FE}:
+tc={00DE00AF-0057-4E3F-82D1-00B600B700D7}:
 tc={00BE0060-0000-4455-9EAE-009D000F0030}:
 tc={00850023-00A4-4C6C-91F2-0047003000C0}:
 tc={00860086-00F3-45F6-9D8A-002F005300A9}:
@@ -655,7 +656,8 @@
     </comment>
     <comment ref="E27" authorId="1" shapeId="0">
       <text>
-        <t xml:space="preserve">tc={007D00EB-001E-4BA6-A456-00B6009B00D7}:
+        <t xml:space="preserve">tc={007C0042-00B3-437D-81D2-006800B200FE}:
+tc={007D00EB-001E-4BA6-A456-00B6009B00D7}:
 tc={005E00E7-006A-462D-8B88-008900BD0099}:
 tc={00590076-0034-4A98-AE21-00B000A1006B}:
 tc={00E4005B-0011-423B-B27E-0061001500D0}:
@@ -669,7 +671,8 @@
     </comment>
     <comment ref="F27" authorId="2" shapeId="0">
       <text>
-        <t xml:space="preserve">tc={005F00F4-00AF-49F8-8A15-000000A100D6}:
+        <t xml:space="preserve">tc={00080025-00F5-428C-82C4-009D00930022}:
+tc={005F00F4-00AF-49F8-8A15-000000A100D6}:
 tc={00E3008D-00A5-4884-B9A4-004500840079}:
 tc={004C0055-0069-4261-A30C-004600BD0064}:
 tc={004400E2-00BB-4E7E-B0CF-0035008A0065}:
@@ -683,7 +686,8 @@
     </comment>
     <comment ref="L27" authorId="3" shapeId="0">
       <text>
-        <t xml:space="preserve">tc={006100BD-0012-4539-8F48-008F002D0066}:
+        <t xml:space="preserve">tc={00840036-00AD-4C98-A488-003100F9007C}:
+tc={006100BD-0012-4539-8F48-008F002D0066}:
 tc={00AA0051-0059-4BCD-A065-006A0083005E}:
 tc={00DD002E-008A-4307-A7A4-004500C900EB}:
 tc={00960062-00C4-4C93-B551-003100B700C6}:
@@ -697,7 +701,8 @@
     </comment>
     <comment ref="M27" authorId="4" shapeId="0">
       <text>
-        <t xml:space="preserve">tc={00EA0038-0068-4F70-B8FC-003B00A30077}:
+        <t xml:space="preserve">tc={00FD0099-0057-486C-8F18-00F400D000FC}:
+tc={00EA0038-0068-4F70-B8FC-003B00A30077}:
 tc={003E0070-0010-43E2-8383-00140050004C}:
 tc={001600B2-008C-4545-84E5-003500660061}:
 tc={0057008B-001A-43DA-9D0E-00BF00E90058}:
@@ -4823,6 +4828,29 @@
     <mergeCell ref="J44:O44"/>
     <mergeCell ref="AL44:AP44"/>
   </mergeCells>
+  <dataValidations count="7">
+    <dataValidation sqref="AJ13:AU41" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Недопустимое значение." error="Такой записи нет в списке" promptTitle="Выбор из списка." prompt="Пожалуйста, выберите  из списка" type="list">
+      <formula1>'&lt;Worksheet "Main"&gt;'!$E$48:$AB$48</formula1>
+    </dataValidation>
+    <dataValidation sqref="AJ13:AU41" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Недопустимое значение." error="Такой записи нет в списке" promptTitle="Выбор из списка." prompt="Пожалуйста, выберите  из списка" type="list">
+      <formula1>'Main'!$E$48:$AB$48</formula1>
+    </dataValidation>
+    <dataValidation sqref="AJ13:AU41" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Недопустимое значение." error="Такой записи нет в списке" promptTitle="Выбор из списка." prompt="Пожалуйста, выберите  из списка" type="list">
+      <formula1>'Main'!$E$48:$AB$48</formula1>
+    </dataValidation>
+    <dataValidation sqref="E13:AI35" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Недопустимое значение." error="Такой записи нет в списке" promptTitle="Выбор из списка." prompt="Пожалуйста, выберите  из списка" type="list">
+      <formula1>'Main'!$E$48:$AB$48</formula1>
+    </dataValidation>
+    <dataValidation sqref="E13:AI35" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Недопустимое значение." error="Такой записи нет в списке" promptTitle="Выбор из списка." prompt="Пожалуйста, выберите  из списка" type="list">
+      <formula1>'Main'!$E$48:$AB$48</formula1>
+    </dataValidation>
+    <dataValidation sqref="E13:AI35" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Недопустимое значение." error="Такой записи нет в списке" promptTitle="Выбор из списка." prompt="Пожалуйста, выберите  из списка" type="list">
+      <formula1>'Main'!$E$48:$AB$48</formula1>
+    </dataValidation>
+    <dataValidation sqref="E13:AI35" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Недопустимое значение." error="Такой записи нет в списке" promptTitle="Выбор времени работы из списка." prompt="Пожалуйста, выберите время работы из списка" type="list">
+      <formula1>'Main'!$E$48:$AB$48</formula1>
+    </dataValidation>
+  </dataValidations>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.6680555555555556" right="0.2590277777777781" top="0.39375" bottom="0.39375" header="0.5118110236220469" footer="0.5118110236220469"/>
   <pageSetup orientation="portrait" paperSize="9" scale="70" fitToHeight="1" fitToWidth="1" useFirstPageNumber="0" pageOrder="downThenOver" usePrinterDefaults="1" blackAndWhite="0" draft="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>